<commit_message>
Adding weights constraints to indexes
</commit_message>
<xml_diff>
--- a/Weights.xlsx
+++ b/Weights.xlsx
@@ -513,16 +513,16 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>0.6315</v>
+        <v>0.5998</v>
       </c>
       <c r="C2">
-        <v>0.0048</v>
+        <v>0.05</v>
       </c>
       <c r="D2">
-        <v>0.3252</v>
+        <v>0.3002</v>
       </c>
       <c r="E2">
-        <v>0.0385</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -530,16 +530,16 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>0.9493</v>
+        <v>0.85</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="E3">
-        <v>0.0507</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -603,28 +603,28 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>0.3183</v>
+        <v>0.2536</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="D2">
-        <v>0.2134</v>
+        <v>0.161</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="F2">
-        <v>0.0944</v>
+        <v>0.0939</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="H2">
-        <v>0.1871</v>
+        <v>0.1631</v>
       </c>
       <c r="I2">
-        <v>0.1867</v>
+        <v>0.1784</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -632,28 +632,28 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>0.65</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -729,28 +729,28 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>0.4058</v>
+        <v>0.3185</v>
       </c>
       <c r="C2">
-        <v>0.0804</v>
+        <v>0.0659</v>
       </c>
       <c r="D2">
-        <v>0.1726</v>
+        <v>0.1297</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="H2">
-        <v>0.3412</v>
+        <v>0.2859</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -758,28 +758,28 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>0.643</v>
+        <v>0.4022</v>
       </c>
       <c r="C3">
-        <v>0.357</v>
+        <v>0.2978</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -855,28 +855,28 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="C2">
-        <v>0.0496</v>
+        <v>0.05</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="E2">
-        <v>0.1912</v>
+        <v>0.1554</v>
       </c>
       <c r="F2">
-        <v>0.4118</v>
+        <v>0.3822</v>
       </c>
       <c r="G2">
-        <v>0.0704</v>
+        <v>0.064</v>
       </c>
       <c r="H2">
-        <v>0.076</v>
+        <v>0.0544</v>
       </c>
       <c r="I2">
-        <v>0.201</v>
+        <v>0.194</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -884,28 +884,28 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>0.3371</v>
+        <v>0.3097</v>
       </c>
       <c r="C3">
-        <v>0.3603</v>
+        <v>0.2894</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="F3">
-        <v>0.3026</v>
+        <v>0.151</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -1256,13 +1256,13 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="C2">
-        <v>0.5904939263525451</v>
+        <v>0.0500000160251316</v>
       </c>
       <c r="D2">
-        <v>5.52531744795898E-16</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1270,13 +1270,13 @@
         <v>20</v>
       </c>
       <c r="B3">
-        <v>2.61554046269033E-16</v>
+        <v>0.05</v>
       </c>
       <c r="C3">
-        <v>1.83789415143846E-17</v>
+        <v>0.0499999999999998</v>
       </c>
       <c r="D3">
-        <v>0.233517691657122</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1284,13 +1284,13 @@
         <v>10</v>
       </c>
       <c r="B4">
-        <v>0.184306516010148</v>
+        <v>0.0500000694278713</v>
       </c>
       <c r="C4">
-        <v>5.03834360223211E-24</v>
+        <v>0.05</v>
       </c>
       <c r="D4">
-        <v>0.176818156685807</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1298,13 +1298,13 @@
         <v>1</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>0.0500000000000001</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1312,13 +1312,13 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>0.0500000000000003</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="D6">
-        <v>0.193276868481642</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1326,13 +1326,13 @@
         <v>2</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="D7">
-        <v>0.151728034674001</v>
+        <v>0.0629489401567271</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1340,13 +1340,13 @@
         <v>16</v>
       </c>
       <c r="B8">
-        <v>1.20927463002283E-17</v>
+        <v>0.05</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>0.0500000000000001</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1354,13 +1354,13 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>0.0499999999999999</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>0.0500000000000001</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>0.0500000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1368,13 +1368,13 @@
         <v>21</v>
       </c>
       <c r="B10">
-        <v>2.37067060980517E-16</v>
+        <v>0.0499999999999999</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>0.0499999999999999</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1382,13 +1382,13 @@
         <v>19</v>
       </c>
       <c r="B11">
-        <v>0.815693483989853</v>
+        <v>0.0999999305721293</v>
       </c>
       <c r="C11">
-        <v>0.361398589516346</v>
+        <v>0.09999998397486889</v>
       </c>
       <c r="D11">
-        <v>8.40632475431135E-17</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1396,13 +1396,13 @@
         <v>18</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="C12">
-        <v>9.64680476789677E-17</v>
+        <v>0.0500000000000001</v>
       </c>
       <c r="D12">
-        <v>7.009774587788309E-18</v>
+        <v>0.0499999999999999</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1410,13 +1410,13 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>0.0500000000000001</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="D13">
-        <v>1.51900324255018E-16</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1424,13 +1424,13 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="C14">
-        <v>3.8466997416824E-17</v>
+        <v>0.05</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1438,13 +1438,13 @@
         <v>3</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="C15">
-        <v>0.0481074841311104</v>
+        <v>0.05</v>
       </c>
       <c r="D15">
-        <v>0.0060431374013035</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1452,13 +1452,13 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>3.55051091632676E-18</v>
+        <v>0.05</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="D16">
-        <v>0.188515240326063</v>
+        <v>0.0870510598432723</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1466,13 +1466,13 @@
         <v>9</v>
       </c>
       <c r="B17">
-        <v>4.83548432374927E-16</v>
+        <v>0.05</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>0.0500000000000002</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1480,13 +1480,13 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>1.25624489605492E-17</v>
+        <v>0.0500000000000001</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="D18">
-        <v>0.0501008707740621</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1494,13 +1494,13 @@
         <v>13</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>0.0500000000000001</v>
       </c>
       <c r="C19">
-        <v>4.21340825322313E-16</v>
+        <v>0.05</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>0.0500000000000001</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1508,13 +1508,13 @@
         <v>15</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="C20">
-        <v>2.55758295292873E-19</v>
+        <v>0.05</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
   </sheetData>
@@ -1839,10 +1839,10 @@
         <v>0.817673754794911</v>
       </c>
       <c r="C2">
-        <v>0.417917676417552</v>
+        <v>0.05</v>
       </c>
       <c r="D2">
-        <v>0.89627570317153</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1853,10 +1853,10 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>5.8742946122691E-17</v>
+        <v>0.05</v>
       </c>
       <c r="D3">
-        <v>1.90960345658245E-17</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1867,10 +1867,10 @@
         <v>0.0245691588433001</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1881,10 +1881,10 @@
         <v>0.0199097404157569</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="D5">
-        <v>5.16855169738481E-20</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1895,10 +1895,10 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <v>2.07366706641342E-17</v>
+        <v>0.05</v>
       </c>
       <c r="D6">
-        <v>6.76351970836212E-18</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1909,10 +1909,10 @@
         <v>0.09277294550444901</v>
       </c>
       <c r="C7">
-        <v>0.260678414207457</v>
+        <v>0.0499999999999996</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1923,10 +1923,10 @@
         <v>0</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1937,10 +1937,10 @@
         <v>1.66620215001128E-17</v>
       </c>
       <c r="C9">
-        <v>9.78975528193244E-18</v>
+        <v>0.0500000000000001</v>
       </c>
       <c r="D9">
-        <v>1.56163560132322E-17</v>
+        <v>0.0500000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1951,10 +1951,10 @@
         <v>0</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>0.0500000000000001</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>0.0499999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1965,10 +1965,10 @@
         <v>2.20236328132266E-20</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1979,10 +1979,10 @@
         <v>0</v>
       </c>
       <c r="C12">
-        <v>8.721529605782819E-18</v>
+        <v>0.05</v>
       </c>
       <c r="D12">
-        <v>4.37737869337174E-18</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1993,10 +1993,10 @@
         <v>0</v>
       </c>
       <c r="C13">
-        <v>2.81585304574087E-17</v>
+        <v>0.0499999999999999</v>
       </c>
       <c r="D13">
-        <v>4.06828638747765E-18</v>
+        <v>0.0499999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -2007,10 +2007,10 @@
         <v>0</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="D14">
-        <v>8.08964679907028E-19</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -2021,10 +2021,10 @@
         <v>0.0336512269104848</v>
       </c>
       <c r="C15">
-        <v>0.0300864083241919</v>
+        <v>0.05</v>
       </c>
       <c r="D15">
-        <v>0.0417686614573752</v>
+        <v>0.0500000000000003</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -2035,10 +2035,10 @@
         <v>0</v>
       </c>
       <c r="C16">
-        <v>5.134140806679499E-19</v>
+        <v>0.05</v>
       </c>
       <c r="D16">
-        <v>1.10174344696643E-17</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -2049,10 +2049,10 @@
         <v>0</v>
       </c>
       <c r="C17">
-        <v>7.42107084232131E-17</v>
+        <v>0.0500000000000001</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>0.0500000000000001</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -2063,10 +2063,10 @@
         <v>1.33841285861342E-18</v>
       </c>
       <c r="C18">
-        <v>0.228313969312479</v>
+        <v>0.09999999999999989</v>
       </c>
       <c r="D18">
-        <v>0.0400810580181304</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -2077,10 +2077,10 @@
         <v>0</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="D19">
-        <v>3.93097832598748E-17</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -2091,10 +2091,10 @@
         <v>0.0114231735310983</v>
       </c>
       <c r="C20">
-        <v>0.06300353173831889</v>
+        <v>0.05</v>
       </c>
       <c r="D20">
-        <v>0.021874577352964</v>
+        <v>0.05</v>
       </c>
     </row>
   </sheetData>
@@ -2129,16 +2129,16 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>0.1881</v>
+        <v>0.1634</v>
       </c>
       <c r="C2">
-        <v>0.6773</v>
+        <v>0.6529</v>
       </c>
       <c r="D2">
-        <v>0.1346</v>
+        <v>0.1338</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -2146,16 +2146,16 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -2207,16 +2207,16 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>0.2791</v>
+        <v>0.2707</v>
       </c>
       <c r="C2">
-        <v>0.1669</v>
+        <v>0.1503</v>
       </c>
       <c r="D2">
-        <v>0.554</v>
+        <v>0.529</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -2224,16 +2224,16 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>0.85</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -2302,16 +2302,16 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>0.85</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -2380,16 +2380,16 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="C3">
-        <v>0.3151</v>
+        <v>0.3058</v>
       </c>
       <c r="D3">
-        <v>0.4834</v>
+        <v>0.4692</v>
       </c>
       <c r="E3">
-        <v>0.2015</v>
+        <v>0.1751</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -2441,16 +2441,16 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>0.9529</v>
+        <v>0.85</v>
       </c>
       <c r="C2">
-        <v>0.0471</v>
+        <v>0.05</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -2458,16 +2458,16 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>0.85</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -2531,28 +2531,28 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>0.8963</v>
+        <v>0.65</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="F2">
-        <v>0.0418</v>
+        <v>0.05</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="H2">
-        <v>0.0401</v>
+        <v>0.05</v>
       </c>
       <c r="I2">
-        <v>0.0219</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -2560,28 +2560,28 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="D3">
-        <v>0.2446</v>
+        <v>0.2146</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="F3">
-        <v>0.0378</v>
+        <v>0.05</v>
       </c>
       <c r="G3">
-        <v>0.3647</v>
+        <v>0.3215</v>
       </c>
       <c r="H3">
-        <v>0.2925</v>
+        <v>0.2138</v>
       </c>
       <c r="I3">
-        <v>0.0604</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -2657,28 +2657,28 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>0.858</v>
+        <v>0.65</v>
       </c>
       <c r="C2">
-        <v>0.0244</v>
+        <v>0.05</v>
       </c>
       <c r="D2">
-        <v>0.0204</v>
+        <v>0.05</v>
       </c>
       <c r="E2">
-        <v>0.0973</v>
+        <v>0.05</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -2686,28 +2686,28 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="C3">
-        <v>0.1843</v>
+        <v>0.05</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="G3">
-        <v>0.8157</v>
+        <v>0.65</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -2783,28 +2783,28 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>0.4577</v>
+        <v>0.3383</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="D2">
-        <v>0.2696</v>
+        <v>0.1939</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="H2">
-        <v>0.0296</v>
+        <v>0.05</v>
       </c>
       <c r="I2">
-        <v>0.2431</v>
+        <v>0.2178</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -2812,28 +2812,28 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>0.5905</v>
+        <v>0.2991</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="F3">
-        <v>0.3614</v>
+        <v>0.4009</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="H3">
-        <v>0.0481</v>
+        <v>0.05</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="4" spans="1:9">

</xml_diff>